<commit_message>
Feat: ultimos cambios del servidor
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -1,61 +1,134 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moren\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B18B53-09E4-40A7-BAA6-506373325AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E2B1E3-CE0D-4C03-8C47-DAECCB1FC2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24B53E22-78E8-4749-89CC-8ACD4B64FDA2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>http://notimx.mx/2023/10/pone-en-marcha-alcalde-adolfo-cerqueda.html</t>
-  </si>
-  <si>
-    <t>http://lado.mx/n.php?id=14387853</t>
-  </si>
-  <si>
-    <t>http://eldiario.com.co/opinion/el-ministro-ivan-velasquez-idoneo-y-digno/</t>
-  </si>
-  <si>
-    <t>http://eltiempo.com/economia/empresas/endeavor-colombia-nombra-a-julio-rojas-sarmiento-como-presidente-de-su-junta-directiva-809861</t>
-  </si>
-  <si>
-    <t>http://elnuevosiglo.com.co/articulos/09-25-2023-impacto-de-economia-en-empresas-frenara-la-caida-del-desempleo</t>
-  </si>
-  <si>
-    <t>http://jota.info/opiniao-e-analise/artigos/o-regulamento-europeu-do-desmatamento-e-efeitos-extraterritoriais-14102023</t>
-  </si>
-  <si>
-    <t>http://revistawhatsup.com/2023/10/xiaomi-anuncia-el-lanzamiento-en.html</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>http://eltiempo.com/opinion/editorial/el-viaje-a-china-editorial-el-tiempo-820252</t>
+  </si>
+  <si>
+    <t>http://lapatria.com/opinion/editoriales/la-mirada-china</t>
+  </si>
+  <si>
+    <t>http://eluniversal.com.co/opinion/columna/a-echar-el-cuento-AB9344471</t>
+  </si>
+  <si>
+    <t>http://cronicadelquindio.com/opinion/opinion/a-echar-el-cuento</t>
+  </si>
+  <si>
+    <t>http://fedegan.org.co/columna-presidente/echar-el-cuento</t>
+  </si>
+  <si>
+    <t>http://billionaires.africa/2023/11/17/south-african-tycoon-gary-nagle-earns-6-1-million-salary-from-glencore-in-2022/</t>
+  </si>
+  <si>
+    <t>http://news.eseuro.com/local/2575336.html</t>
+  </si>
+  <si>
+    <t>http://fr.eseuro.com/local/1228558.html</t>
+  </si>
+  <si>
+    <t>http://globalarbitrationreview.com/article/glencore-brings-new-claim-against-colombia</t>
+  </si>
+  <si>
+    <t>http://newstodayjournal.com/the-kidnap-of-liverpool-footballer-luis-diazs-father-as-told-by-his-family/</t>
+  </si>
+  <si>
+    <t>http://elespectador.com/opinion/columnistas/columnista-invitado-ee/lo-que-le-leo-a-mi-hijo-cuando-el-mundo-esta-en-llamas/</t>
+  </si>
+  <si>
+    <t>http://elcolombiano.com/opinion/editoriales/guia-para-descuadernar-la-economia-KD23138525</t>
+  </si>
+  <si>
+    <t>http://laopinion.com.co/editorial/billonaria-derrota</t>
+  </si>
+  <si>
+    <t>http://ecosdelcombeima.com/columnista/nota-233004-de-las-ideas-los-hechos-menos-analisis-mas-accion</t>
+  </si>
+  <si>
+    <t>http://opanoticias.com/Opinion/democracia-ambiental/31992</t>
+  </si>
+  <si>
+    <t>http://revistalaregion.com/index.php/es/sociedad/item/11812-final-fear-the-walking-dead-este-lunes-en-colombia</t>
+  </si>
+  <si>
+    <t>http://noticiasyrespuestas.com/2023/11/18/llega-en-vivo-miss-universo-2023-conozca-las-mujeres-que-representan-a-latinoamerica/</t>
+  </si>
+  <si>
+    <t>http://elespectador.com/entretenimiento/taylor-swift-pospone-concierto-de-este-sabado-en-rio-de-janeiro-por-temperaturas-extremas/</t>
+  </si>
+  <si>
+    <t>http://elpais.com.co/politica/nayib-bukele-le-lanzo-dura-respuesta-a-petro-por-lamentar-triunfo-de-javier-milei-en-argentina-1921.html</t>
+  </si>
+  <si>
+    <t>http://vanguardia.com/economia/nacional/desde-el-ministerio-de-vivienda-se-lanzo-nuevo-plan-para-la-construccion-de-viviendas-sociales-BB8003210</t>
+  </si>
+  <si>
+    <t>http://diariodelsur.com.co/mindefensa-coordina-temas-de-seguridad-frente-a-la-reunion-de-colombia-con-venezuela/</t>
+  </si>
+  <si>
+    <t>http://semana.com/confidenciales/articulo/arruinan-a-ecopetrol-al-asociarla-con-pdvsa-alvaro-uribe/202304/</t>
+  </si>
+  <si>
+    <t>http://msn.com/es-co/noticias/other/partidos-para-hoy-domingo-19-de-noviembre-liga-mx-femenil-expansi%C3%B3n-mx-y-m%C3%A1s/ar-AA1kbsPr</t>
+  </si>
+  <si>
+    <t>http://las2orillas.co/los-empresarios-que-no-se-robaron-la-plata-como-centros-poblados-han-llevado-internet-a-6-700-pueblos/</t>
+  </si>
+  <si>
+    <t>http://semana.com/deportes/articulo/historial-de-chipi-chipi-castillo-lo-complica-revelan-lios-pasados-del-jugador-de-nacional-en-medio-de-escandalo/202336/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,16 +151,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -101,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -117,7 +204,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -129,7 +216,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -176,6 +263,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -211,6 +315,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -362,55 +483,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13C56DF-697A-4055-92C2-9818CCB489A1}">
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="126.88671875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" display="https://www.msn.com/es-co/noticias/other/partidos-para-hoy-domingo-19-de-noviembre-liga-mx-femenil-expansi%C3%B3n-mx-y-m%C3%A1s/ar-AA1kbsPr" xr:uid="{DAF451C3-27AC-4B8A-AEC4-79FB1DF7278A}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://noticiasyrespuestas.com/2023/11/18/llega-en-vivo-miss-universo-2023-conozca-las-mujeres-que-representan-a-latinoamerica/" xr:uid="{C306B656-2817-4931-9210-7726060D0FAA}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://www.semana.com/deportes/articulo/historial-de-chipi-chipi-castillo-lo-complica-revelan-lios-pasados-del-jugador-de-nacional-en-medio-de-escandalo/202336/" xr:uid="{BD41B9C7-AAB5-4CD2-A056-675109C2FF39}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>